<commit_message>
updated benchmark data and added library files
</commit_message>
<xml_diff>
--- a/benchmark/assesment/Qwark_Benchmarks.xlsx
+++ b/benchmark/assesment/Qwark_Benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiram-AW\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB8949F-7918-452C-BD0D-0C288C542449}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428FD613-93AF-4592-94AA-2E61E59B1432}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="954" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="954" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original C" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>System Checkpoint</t>
   </si>
@@ -175,9 +175,6 @@
     <t>O2*</t>
   </si>
   <si>
-    <t xml:space="preserve">OpenMSP430 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Qwark </t>
   </si>
   <si>
@@ -201,15 +198,60 @@
   <si>
     <t>Cuckoo 10 ms</t>
   </si>
+  <si>
+    <t>Qwark Checkpoints</t>
+  </si>
+  <si>
+    <t>NV-Qwark Checkpoints</t>
+  </si>
+  <si>
+    <t>Qwark ms</t>
+  </si>
+  <si>
+    <t>NV-Qwark cycles</t>
+  </si>
+  <si>
+    <t>Qwark cycles</t>
+  </si>
+  <si>
+    <t>OpenMSP430 cycles</t>
+  </si>
+  <si>
+    <t>NV-Qwark ms</t>
+  </si>
+  <si>
+    <t>NV-Qwark s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NV-Qwark </t>
+  </si>
+  <si>
+    <t>1.262 s</t>
+  </si>
+  <si>
+    <t>78.3105 ms</t>
+  </si>
+  <si>
+    <t>29.956 ms</t>
+  </si>
+  <si>
+    <t>1.315 s</t>
+  </si>
+  <si>
+    <t>77.675 ms</t>
+  </si>
+  <si>
+    <t>31.120 ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -235,8 +277,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,8 +328,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -282,12 +343,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -316,11 +406,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -328,7 +445,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="24">
     <dxf>
       <font>
         <b val="0"/>
@@ -341,7 +458,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -360,7 +477,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -379,7 +496,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -398,7 +515,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -417,7 +534,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -436,7 +553,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -455,7 +572,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -474,7 +591,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -493,7 +610,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -512,7 +629,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -531,7 +648,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -550,7 +667,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -569,12 +686,22 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -588,7 +715,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -597,7 +724,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -607,406 +734,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -3632,7 +3360,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Checkpoints</c:v>
+                  <c:v>Qwark Checkpoints</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3768,6 +3496,151 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-00DE-48C1-BA52-8E31E46C1B06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark AR'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark Checkpoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Qwark Bitcount'!$D$2:$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>O0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>O1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O0*</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>O1*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>O2*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark Bitcount'!$K$2:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E90E-4EF1-BD17-3635AD77A24B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4144,7 +4017,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>OpenMSP430 </c:v>
+                  <c:v>OpenMSP430 cycles</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4167,63 +4040,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Qwark Bitcount'!$D$2:$D$7</c:f>
@@ -4292,7 +4108,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Qwark </c:v>
+                  <c:v>Qwark cycles</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4315,63 +4131,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Qwark Bitcount'!$D$2:$D$7</c:f>
@@ -4431,10 +4190,120 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark AR'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark cycles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Qwark Bitcount'!$D$2:$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>O0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>O1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O0*</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>O1*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>O2*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark Bitcount'!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>835373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>358306</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>333763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>873509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>373593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>349682</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A62-42CE-B4D9-B4A539D164E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -4452,61 +4321,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>OPTIMIZATION LEVEL</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4572,66 +4386,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>EXECUTION TIME</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (CYCLES)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4863,88 +4617,32 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'Qwark AR'!$D$2:$D$7</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>'Qwark AR'!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>O0</c:v>
+                  <c:v>24205000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>O1</c:v>
+                  <c:v>5349000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>O2</c:v>
+                  <c:v>4609000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>O0*</c:v>
+                  <c:v>25168000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>O1*</c:v>
+                  <c:v>5579353</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>O2*</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>4798903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -5011,88 +4709,32 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'Qwark AR'!$D$2:$D$7</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>'Qwark AR'!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>O0</c:v>
+                  <c:v>24205000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>O1</c:v>
+                  <c:v>5349000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>O2</c:v>
+                  <c:v>4609000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>O0*</c:v>
+                  <c:v>25168000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>O1*</c:v>
+                  <c:v>5579353</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>O2*</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>4798903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -5127,10 +4769,95 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark AR'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark cycles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark AR'!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24205000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5349000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4609000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25168000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5579353</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4798903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7185-42A8-B96E-A68FD0D27ACA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5552,64 +5279,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Qwark AR'!$D$2:$D$7</c:f>
@@ -5669,10 +5338,67 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark AR'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark Checkpoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark AR'!$K$2:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>57789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9742</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7766</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2703-47F7-BE6C-8989E4E606FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -6065,63 +5791,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Qwark Cuckoo'!$D$2:$D$7</c:f>
@@ -6213,63 +5882,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Qwark Cuckoo'!$D$2:$D$7</c:f>
@@ -6329,10 +5941,95 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark Cuckoo'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark cycles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark Cuckoo'!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1262000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29956</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1315000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA2C-4B95-85A0-8E334B530AE7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -6860,6 +6557,121 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5B1C-4A1D-8315-688C4C34AEAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Qwark Cuckoo'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NV-Qwark Checkpoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Qwark Cuckoo'!$K$2:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2735</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8093-4FEC-BF85-6EB55B3C5F00}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12279,7 +12091,7 @@
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="7231380" y="1524000"/>
+    <xdr:pos x="7100751" y="3069771"/>
     <xdr:ext cx="5036820" cy="3703320"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12307,7 +12119,7 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
   <xdr:absoluteAnchor>
-    <xdr:pos x="1196340" y="1546860"/>
+    <xdr:pos x="1141912" y="3081746"/>
     <xdr:ext cx="5753100" cy="3729370"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12340,7 +12152,7 @@
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="918210" y="2011680"/>
+    <xdr:pos x="918210" y="2666104"/>
     <xdr:ext cx="6366510" cy="3484778"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12368,8 +12180,8 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
   <xdr:absoluteAnchor>
-    <xdr:pos x="7299960" y="1965960"/>
-    <xdr:ext cx="4077054" cy="3218830"/>
+    <xdr:pos x="7634855" y="2719956"/>
+    <xdr:ext cx="4350315" cy="3386930"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2">
@@ -12401,7 +12213,7 @@
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="681989" y="1501140"/>
+    <xdr:pos x="714646" y="2459083"/>
     <xdr:ext cx="6000751" cy="3151403"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12429,8 +12241,8 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
   <xdr:absoluteAnchor>
-    <xdr:pos x="6781800" y="1508760"/>
-    <xdr:ext cx="4922874" cy="3150250"/>
+    <xdr:pos x="7434943" y="2434045"/>
+    <xdr:ext cx="5007428" cy="3150325"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2">
@@ -12460,72 +12272,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A888757F-F360-479A-B692-B7D51EC62C5C}" name="Tabla1" displayName="Tabla1" ref="A6:F18" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A888757F-F360-479A-B692-B7D51EC62C5C}" name="Tabla1" displayName="Tabla1" ref="A6:F18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A6:F18" xr:uid="{1056625E-8206-4C48-B6EB-BD8212CEEB43}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4981DE85-F7A0-4B16-B6FB-304A8B6F0EBE}" name="Clock" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{BFCC6651-2FD4-4748-9865-4E87AE7A6848}" name="1 MHz" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{1C313214-6C7C-4A12-9537-5CE9F6FFF671}" name="Columna1" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{4AD15C24-12D1-4A26-BAFB-375C81006DDD}" name="Columna2" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{FEF5753D-B565-4272-83C6-1E2803CA983C}" name="Columna3" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{C801A8B9-D3CD-4F49-B4E0-F982D028C749}" name="Columna4" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{4981DE85-F7A0-4B16-B6FB-304A8B6F0EBE}" name="Clock" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{BFCC6651-2FD4-4748-9865-4E87AE7A6848}" name="1 MHz" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{1C313214-6C7C-4A12-9537-5CE9F6FFF671}" name="Columna1" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{4AD15C24-12D1-4A26-BAFB-375C81006DDD}" name="Columna2" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{FEF5753D-B565-4272-83C6-1E2803CA983C}" name="Columna3" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{C801A8B9-D3CD-4F49-B4E0-F982D028C749}" name="Columna4" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9FF1F8D2-E98F-49E5-93F3-7F1D14CCFDFF}" name="Tabla2" displayName="Tabla2" ref="B1:K7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="B1:K7" xr:uid="{509A76D4-2335-4D62-A485-D59BCA64C4BD}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{FBF25D7B-2CD2-4CD3-8C63-DE2B27EF0577}" name="Benchmark" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{87E9E989-274E-4105-A0F7-A2464CC96D42}" name="Compiler" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{662464B7-1006-47B3-854E-41DC40A034A5}" name="Optimization" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{6FB2993A-3E29-4EC8-A7EC-E212934FF279}" name="OpenMSP430 " dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{88A6F6E0-6AC5-4174-8589-09D2E9B8B7FE}" name="Qwark " dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{508BCE4B-2E85-41E7-A54A-3C92D0EFFDD7}" name="ms" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{3998AA0F-5286-4A46-A125-EE328BF58E29}" name="Checkpoints" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{E12F4210-0681-476D-BD4E-AE3E1CB995A5}" name="Read Buffer Length" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{41019993-C61A-4AB6-81A2-25531CD4E7D5}" name="Write Buffer Length" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{C7390D51-4433-43FD-AC5B-7B3CC6917B4D}" name="TLB buffer Length" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B47B3E52-00B7-4AB0-A039-D0426E6241D0}" name="Tabla3" displayName="Tabla3" ref="B1:K7" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B1:K7" xr:uid="{EB3EE55D-9167-4AA4-A526-763D91BDEE31}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{603CF8AE-3526-463B-92DA-AC27A14A38F6}" name="Benchmark" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{BBB4B4F6-CFD0-43E3-8219-F9A9EFC3CA5B}" name="Compiler" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A764F0D8-D633-4BE9-93E2-54008E14CDD3}" name="Optimization" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{2656A178-FBDA-463A-B796-71C98CE575D7}" name="OpenMSP430" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{C8673E4A-0E5F-4534-8F8C-AEFFEA01FDFC}" name="Qwark " dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{A6BF1D55-02C7-418A-809F-CD6EBE60E6B6}" name="s" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{072D3936-40E3-491C-B417-884C2C8840BA}" name="Checkpoints" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F7E7D031-A7D3-4E8E-A61C-672EB2292697}" name="Read Buffer Length" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{7CA5F096-1873-4B8D-82F4-641D8EAB46D8}" name="Write Buffer Length" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{CB29CFB6-A2EB-4575-AEDE-1FCF7CDA040D}" name="TLB buffer Length" dataDxfId="13"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2F4A806D-EFB9-427C-B0B2-6EE82AEE08B2}" name="Tabla4" displayName="Tabla4" ref="B1:K7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B1:K7" xr:uid="{7EA62A81-E9E8-456B-BD85-A8D4AD0315C5}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{6E62DFC2-9010-449E-BCED-D77991AB40C1}" name="Benchmark" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{6D03B423-68AD-4F1A-A2F1-1DCE65DF3F1A}" name="Compiler" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{4DF18005-25BB-4E48-864C-8DA2F2616683}" name="Optimization" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A44E283B-A3EA-40FE-BB3B-AC580588EBE6}" name="OpenMSP430" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C63A2ED8-4184-4480-B069-FDFC19489480}" name="Qwark" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{82074883-5D48-4862-863E-266557FD3638}" name="ms" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5FFC81AA-2966-4F16-8B01-C13C6245A3DC}" name="Checkpoints" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{579F909A-6BBF-4279-9C5D-F2385A268020}" name="Read Buffer Length" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{655D3EC0-FB3C-443E-80FE-D9769596E83A}" name="Write Buffer Length" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{8C362058-5113-4AB4-863C-0054A70B4041}" name="TLB buffer Length" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{24EFC539-526E-4C9E-96A6-6E9BA1808CAB}" name="Tabla6" displayName="Tabla6" ref="B1:N7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="B1:N7" xr:uid="{2C5D8F62-E429-48EB-86AD-EDD255C7F1DE}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{B21C40C3-8A7F-475D-9DA6-A87147DD3AF8}" name="Benchmark" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{620DA34A-E142-4A18-974D-A75B8E1E512C}" name="Compiler" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{7E8D08E0-9005-4EBB-84C3-87B5C4C15806}" name="Optimization" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{8F5A333F-5D62-46A9-9BC1-A315F6C05D6C}" name="OpenMSP430 cycles" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{570BC2EF-4E49-42BE-A16F-D3526625A6BF}" name="Qwark cycles" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{9BBB93C4-C84F-49A1-A328-ECAE35C7A274}" name="Qwark ms" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{65765902-EA91-4D82-9722-C70951262262}" name="Qwark Checkpoints" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{DB67D5A7-5DC8-4FD9-9133-1FAE421825A6}" name="NV-Qwark cycles" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{36135582-868F-404A-933B-FBCB90D8D777}" name="NV-Qwark ms" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{5991BFCA-1970-400E-883C-686FEB09B063}" name="NV-Qwark Checkpoints" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{6B19E418-4D08-4661-A72F-F41A12D2F1B3}" name="Read Buffer Length" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BB2D8DB1-FC65-46DA-AA10-82A0403165CC}" name="Write Buffer Length" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{236FF60D-5710-422F-81AE-722D13150411}" name="TLB buffer Length" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12830,8 +12607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="C11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12859,16 +12636,16 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -13104,10 +12881,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13118,240 +12895,310 @@
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="31.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="1026" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="11" width="23.77734375" customWidth="1"/>
+    <col min="12" max="12" width="25.6640625" customWidth="1"/>
+    <col min="13" max="13" width="24.5546875" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="16" max="1029" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="18">
         <v>248710</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="18">
         <v>282601</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="18">
         <v>282.601</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="18">
         <v>93</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="18">
+        <v>835373</v>
+      </c>
+      <c r="J2" s="18">
+        <v>835.37300000000005</v>
+      </c>
+      <c r="K2" s="18">
+        <v>1467</v>
+      </c>
+      <c r="L2" s="18">
         <v>8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="M2" s="18">
         <v>8</v>
       </c>
-      <c r="K2" s="4">
+      <c r="N2" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="17">
         <v>177400</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="17">
         <v>214177</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="17">
         <v>214.17699999999999</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="17">
         <v>92</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="17">
+        <v>358306</v>
+      </c>
+      <c r="J3" s="17">
+        <v>358.30599999999998</v>
+      </c>
+      <c r="K3" s="17">
+        <v>480</v>
+      </c>
+      <c r="L3" s="17">
         <v>8</v>
       </c>
-      <c r="J3" s="4">
+      <c r="M3" s="17">
         <v>8</v>
       </c>
-      <c r="K3" s="4">
+      <c r="N3" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="16">
         <v>170469</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="16">
         <v>211072</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="16">
         <v>210.709</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="16">
         <v>91</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="16">
+        <v>333763</v>
+      </c>
+      <c r="J4" s="16">
+        <v>333.76299999999998</v>
+      </c>
+      <c r="K4" s="16">
+        <v>424</v>
+      </c>
+      <c r="L4" s="16">
         <v>8</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M4" s="16">
         <v>8</v>
       </c>
-      <c r="K4" s="4">
+      <c r="N4" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="17">
         <v>248710</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="17">
         <v>294713</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="17">
         <v>294.71300000000002</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="17">
         <v>115</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="17">
+        <v>873509</v>
+      </c>
+      <c r="J5" s="17">
+        <v>873.50900000000001</v>
+      </c>
+      <c r="K5" s="17">
+        <v>1557</v>
+      </c>
+      <c r="L5" s="17">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="M5" s="17">
         <v>8</v>
       </c>
-      <c r="K5" s="4">
+      <c r="N5" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="16">
         <v>177400</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="16">
         <v>223884</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="16">
         <v>223.88399999999999</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="16">
         <v>115</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="16">
+        <v>373593</v>
+      </c>
+      <c r="J6" s="16">
+        <v>373.59300000000002</v>
+      </c>
+      <c r="K6" s="16">
+        <v>526</v>
+      </c>
+      <c r="L6" s="16">
         <v>8</v>
       </c>
-      <c r="J6" s="4">
+      <c r="M6" s="16">
         <v>8</v>
       </c>
-      <c r="K6" s="4">
+      <c r="N6" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="20">
         <v>170469</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="20">
         <v>221308</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="20">
         <v>221.30799999999999</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="20">
         <v>110</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="20">
+        <v>349682</v>
+      </c>
+      <c r="J7" s="20">
+        <v>349.68200000000002</v>
+      </c>
+      <c r="K7" s="20">
+        <v>468</v>
+      </c>
+      <c r="L7" s="20">
         <v>8</v>
       </c>
-      <c r="J7" s="4">
+      <c r="M7" s="20">
         <v>8</v>
       </c>
-      <c r="K7" s="4">
+      <c r="N7" s="20">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -13369,10 +13216,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:K7"/>
+  <dimension ref="B1:N7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13385,234 +13232,300 @@
     <col min="6" max="6" width="14.109375" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="1026" width="9.109375" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="16" max="1029" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="18">
         <v>3921000</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="18">
         <v>5402326</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="18">
         <v>5.4020000000000001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="18">
         <v>2376</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="18">
+        <v>24205000</v>
+      </c>
+      <c r="J2" s="18">
+        <v>24.204999999999998</v>
+      </c>
+      <c r="K2" s="18">
+        <v>57789</v>
+      </c>
+      <c r="L2" s="18">
         <v>8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="M2" s="18">
         <v>8</v>
       </c>
-      <c r="K2" s="4">
+      <c r="N2" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="17">
         <v>2089016</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="17">
         <v>3154367</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="17">
         <v>3.1539999999999999</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="17">
         <v>2088</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="17">
+        <v>5349000</v>
+      </c>
+      <c r="J3" s="17">
+        <v>5.3490000000000002</v>
+      </c>
+      <c r="K3" s="17">
+        <v>9107</v>
+      </c>
+      <c r="L3" s="17">
         <v>8</v>
       </c>
-      <c r="J3" s="4">
+      <c r="M3" s="17">
         <v>8</v>
       </c>
-      <c r="K3" s="4">
+      <c r="N3" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="16">
         <v>2030978</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="16">
         <v>3257835</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="16">
         <v>3.2570000000000001</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="16">
         <v>2088</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="16">
+        <v>4609000</v>
+      </c>
+      <c r="J4" s="16">
+        <v>4.609</v>
+      </c>
+      <c r="K4" s="16">
+        <v>7251</v>
+      </c>
+      <c r="L4" s="16">
         <v>8</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M4" s="16">
         <v>8</v>
       </c>
-      <c r="K4" s="4">
+      <c r="N4" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="17">
         <v>3921000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="17">
         <v>5722708</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="17">
         <v>5.7220000000000004</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="17">
         <v>2767</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="17">
+        <v>25168000</v>
+      </c>
+      <c r="J5" s="17">
+        <v>25.167999999999999</v>
+      </c>
+      <c r="K5" s="17">
+        <v>60214</v>
+      </c>
+      <c r="L5" s="17">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="M5" s="17">
         <v>8</v>
       </c>
-      <c r="K5" s="4">
+      <c r="N5" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="16">
         <v>2089016</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="16">
         <v>3330410</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="16">
         <v>3.33</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="16">
         <v>2372</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="16">
+        <v>5579353</v>
+      </c>
+      <c r="J6" s="16">
+        <v>5.5789999999999997</v>
+      </c>
+      <c r="K6" s="16">
+        <v>9742</v>
+      </c>
+      <c r="L6" s="16">
         <v>8</v>
       </c>
-      <c r="J6" s="4">
+      <c r="M6" s="16">
         <v>8</v>
       </c>
-      <c r="K6" s="4">
+      <c r="N6" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="22">
         <v>2030978</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="22">
         <v>3455091</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="22">
         <v>3.45</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="22">
         <v>2377</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="22">
+        <v>4798903</v>
+      </c>
+      <c r="J7" s="22">
+        <v>4.798</v>
+      </c>
+      <c r="K7" s="22">
+        <v>7766</v>
+      </c>
+      <c r="L7" s="22">
         <v>8</v>
       </c>
-      <c r="J7" s="4">
+      <c r="M7" s="22">
         <v>8</v>
       </c>
-      <c r="K7" s="4">
+      <c r="N7" s="22">
         <v>8</v>
       </c>
     </row>
@@ -13624,18 +13537,15 @@
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:K14"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13646,251 +13556,318 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="28.109375" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="8" width="14.109375" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" customWidth="1"/>
-    <col min="12" max="1026" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="19.77734375" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" customWidth="1"/>
+    <col min="15" max="1029" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="18">
         <v>316789</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="18">
         <v>327133</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="18">
         <v>327.13299999999998</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="18">
         <v>20</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="18">
+        <v>1262000</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="18">
+        <v>2599</v>
+      </c>
+      <c r="L2" s="18">
         <v>8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="M2" s="18">
         <v>8</v>
       </c>
-      <c r="K2" s="4">
+      <c r="N2" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="17">
         <v>42942</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="17">
         <v>53152</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="24">
         <v>53.152799999999999</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="17">
         <v>20</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="17">
+        <v>78310</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="17">
+        <v>94</v>
+      </c>
+      <c r="L3" s="17">
         <v>8</v>
       </c>
-      <c r="J3" s="4">
+      <c r="M3" s="17">
         <v>8</v>
       </c>
-      <c r="K3" s="4">
+      <c r="N3" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="16">
         <v>11781</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="16">
         <v>20936</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="25">
         <v>20.936499999999999</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="16">
         <v>20</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="16">
+        <v>29956</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="16">
+        <v>47</v>
+      </c>
+      <c r="L4" s="16">
         <v>8</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M4" s="16">
         <v>8</v>
       </c>
-      <c r="K4" s="4">
+      <c r="N4" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="17">
         <v>316789</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="17">
         <v>336024</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="17">
         <v>336.024</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="17">
         <v>40</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="17">
+        <v>1315000</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2735</v>
+      </c>
+      <c r="L5" s="17">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="M5" s="17">
         <v>8</v>
       </c>
-      <c r="K5" s="4">
+      <c r="N5" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="16">
         <v>42942</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="16">
         <v>56389</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="16">
         <v>56.389699999999998</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="16">
         <v>26</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="16">
+        <v>77675</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="16">
+        <v>92</v>
+      </c>
+      <c r="L6" s="16">
         <v>8</v>
       </c>
-      <c r="J6" s="4">
+      <c r="M6" s="16">
         <v>8</v>
       </c>
-      <c r="K6" s="4">
+      <c r="N6" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="22">
         <v>11781</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="22">
         <v>22084</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="22">
         <v>22.084</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="22">
         <v>22</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="22">
+        <v>31120</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="22">
+        <v>50</v>
+      </c>
+      <c r="L7" s="22">
         <v>8</v>
       </c>
-      <c r="J7" s="4">
+      <c r="M7" s="22">
         <v>8</v>
       </c>
-      <c r="K7" s="4">
+      <c r="N7" s="22">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G10" s="15"/>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G11" s="16"/>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G12" s="15"/>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G13" s="16"/>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G14" s="15"/>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -13900,9 +13877,6 @@
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>